<commit_message>
sample data revised (team capacity)
</commit_message>
<xml_diff>
--- a/input/bay_config.xlsx
+++ b/input/bay_config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\young\PycharmProjects\2025_MAS_KSOE\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35502C34-F860-4C59-B64E-60FF895ACBAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E054B0-7315-47C0-94C3-857AC8CE6042}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{F983E655-1C09-4649-8274-FFD858F2B011}"/>
+    <workbookView xWindow="6930" yWindow="5385" windowWidth="28800" windowHeight="15345" xr2:uid="{F983E655-1C09-4649-8274-FFD858F2B011}"/>
   </bookViews>
   <sheets>
     <sheet name="bays" sheetId="2" r:id="rId1"/>
@@ -206,7 +206,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,6 +236,21 @@
       <color rgb="FFFF0000"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -272,13 +287,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -615,11 +630,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7623A047-7E38-46EF-AFE3-6D9377A675D6}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="11.125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.75" style="1" bestFit="1" customWidth="1"/>
@@ -633,7 +648,7 @@
     <col min="11" max="11" width="18.75" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -643,10 +658,10 @@
       <c r="C1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="4" t="s">
         <v>35</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -668,7 +683,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -678,10 +693,10 @@
       <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="5">
         <v>1900</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="5">
         <v>1300</v>
       </c>
       <c r="F2" s="1">
@@ -703,7 +718,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -713,10 +728,10 @@
       <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="5">
         <v>1700</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="5">
         <v>1800</v>
       </c>
       <c r="F3" s="1">
@@ -738,7 +753,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -748,10 +763,10 @@
       <c r="C4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="5">
         <v>8200</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="5">
         <v>12800</v>
       </c>
       <c r="F4" s="1">
@@ -763,17 +778,17 @@
       <c r="H4" s="1">
         <v>20.5</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="3">
         <v>100</v>
       </c>
       <c r="J4" s="1">
         <v>52</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K4" s="3">
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -783,11 +798,11 @@
       <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="4">
-        <v>5000</v>
-      </c>
-      <c r="E5" s="4">
-        <v>5000</v>
+      <c r="D5" s="5">
+        <v>4500</v>
+      </c>
+      <c r="E5" s="5">
+        <v>3500</v>
       </c>
       <c r="F5" s="1">
         <v>16</v>
@@ -808,7 +823,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -818,10 +833,10 @@
       <c r="C6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="5">
         <v>900</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="5">
         <v>900</v>
       </c>
       <c r="F6" s="1">
@@ -843,7 +858,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -853,11 +868,11 @@
       <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="4">
-        <v>5000</v>
-      </c>
-      <c r="E7" s="4">
-        <v>5000</v>
+      <c r="D7" s="5">
+        <v>1300</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1200</v>
       </c>
       <c r="F7" s="1">
         <v>17</v>
@@ -878,7 +893,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -888,11 +903,11 @@
       <c r="C8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="4">
-        <v>5000</v>
-      </c>
-      <c r="E8" s="4">
-        <v>5000</v>
+      <c r="D8" s="5">
+        <v>1200</v>
+      </c>
+      <c r="E8" s="5">
+        <v>1300</v>
       </c>
       <c r="F8" s="1">
         <v>17</v>
@@ -913,7 +928,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -923,10 +938,10 @@
       <c r="C9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="5">
         <v>1700</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="5">
         <v>1900</v>
       </c>
       <c r="F9" s="1">
@@ -948,7 +963,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -958,10 +973,10 @@
       <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="5">
         <v>1799.85</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="5">
         <v>1900</v>
       </c>
       <c r="F10" s="1">
@@ -983,7 +998,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -993,11 +1008,11 @@
       <c r="C11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="4">
-        <v>5000</v>
-      </c>
-      <c r="E11" s="4">
-        <v>5000</v>
+      <c r="D11" s="5">
+        <v>1200</v>
+      </c>
+      <c r="E11" s="5">
+        <v>1200</v>
       </c>
       <c r="F11" s="1">
         <v>23</v>
@@ -1018,7 +1033,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1028,11 +1043,11 @@
       <c r="C12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D12" s="4">
-        <v>5000</v>
-      </c>
-      <c r="E12" s="4">
-        <v>5000</v>
+      <c r="D12" s="5">
+        <v>1500</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1700</v>
       </c>
       <c r="F12" s="1">
         <v>23</v>
@@ -1053,7 +1068,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1063,11 +1078,11 @@
       <c r="C13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="4">
-        <v>5000</v>
-      </c>
-      <c r="E13" s="4">
-        <v>5000</v>
+      <c r="D13" s="5">
+        <v>2100</v>
+      </c>
+      <c r="E13" s="5">
+        <v>2100</v>
       </c>
       <c r="F13" s="1">
         <v>23</v>
@@ -1088,7 +1103,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1098,10 +1113,10 @@
       <c r="C14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="5">
         <v>2700</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="5">
         <v>3000</v>
       </c>
       <c r="F14" s="1">
@@ -1123,7 +1138,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
@@ -1133,11 +1148,11 @@
       <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="4">
-        <v>5000</v>
-      </c>
-      <c r="E15" s="4">
-        <v>5000</v>
+      <c r="D15" s="5">
+        <v>1700</v>
+      </c>
+      <c r="E15" s="5">
+        <v>2100</v>
       </c>
       <c r="F15" s="1">
         <v>27</v>
@@ -1158,7 +1173,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1168,11 +1183,11 @@
       <c r="C16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="4">
-        <v>5000</v>
-      </c>
-      <c r="E16" s="4">
-        <v>5000</v>
+      <c r="D16" s="5">
+        <v>1300</v>
+      </c>
+      <c r="E16" s="5">
+        <v>1500</v>
       </c>
       <c r="F16" s="1">
         <v>27</v>
@@ -1193,7 +1208,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
@@ -1203,11 +1218,11 @@
       <c r="C17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="4">
-        <v>5000</v>
-      </c>
-      <c r="E17" s="4">
-        <v>5000</v>
+      <c r="D17" s="5">
+        <v>2000</v>
+      </c>
+      <c r="E17" s="5">
+        <v>1600</v>
       </c>
       <c r="F17" s="1">
         <v>20</v>
@@ -1228,7 +1243,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -1238,11 +1253,11 @@
       <c r="C18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="4">
-        <v>5000</v>
-      </c>
-      <c r="E18" s="4">
-        <v>5000</v>
+      <c r="D18" s="5">
+        <v>1800</v>
+      </c>
+      <c r="E18" s="5">
+        <v>1700</v>
       </c>
       <c r="F18" s="1">
         <v>20</v>
@@ -1263,7 +1278,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11">
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1271,39 +1286,37 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11">
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11">
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11">
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11">
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11">
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-      <c r="M29" s="1"/>
-      <c r="N29" s="1"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:11">
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>

</xml_diff>